<commit_message>
fix excel 3jr/H=1 credit
</commit_message>
<xml_diff>
--- a/doc/Projet_libre_decoupage_tache.xlsx
+++ b/doc/Projet_libre_decoupage_tache.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeyvo/EPITECH/Projet Libre/PBRaytracer/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CDB30C-EEDF-2645-A786-4E441094992D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D33D7FD-8296-6746-BD65-B6B10CC53136}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{39DAB752-344B-9C46-BDE4-193F0B1E6DAC}"/>
+    <workbookView xWindow="10200" yWindow="2000" windowWidth="18600" windowHeight="14560" xr2:uid="{39DAB752-344B-9C46-BDE4-193F0B1E6DAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -344,7 +344,7 @@
     <tableColumn id="4" xr3:uid="{1C29566B-021E-4847-A43C-BA9A304594FB}" name="Tâche fonctionnelle" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{089EF323-C7BA-0F4F-AE31-612C56D94DBA}" name="Charge de travail (en jour/Homme)" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{98E21285-F6C2-5141-97EE-6DD5D126E215}" name="Crédit" dataDxfId="0">
-      <calculatedColumnFormula>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</calculatedColumnFormula>
+      <calculatedColumnFormula>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A726377-1964-D341-8EAE-D95ECF1DA9DA}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,8 +699,8 @@
         <v>1</v>
       </c>
       <c r="F2" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>0.5</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -718,8 +718,8 @@
         <v>2</v>
       </c>
       <c r="F3" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -737,8 +737,8 @@
         <v>2</v>
       </c>
       <c r="F4" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -756,8 +756,8 @@
         <v>2</v>
       </c>
       <c r="F5" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -775,8 +775,8 @@
         <v>3</v>
       </c>
       <c r="F6" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1.5</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -794,8 +794,8 @@
         <v>3</v>
       </c>
       <c r="F7" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1.5</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -813,8 +813,8 @@
         <v>3</v>
       </c>
       <c r="F8" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1.5</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -832,8 +832,8 @@
         <v>3</v>
       </c>
       <c r="F9" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1.5</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -851,8 +851,8 @@
         <v>2</v>
       </c>
       <c r="F10" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -870,8 +870,8 @@
         <v>1</v>
       </c>
       <c r="F11" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>0.5</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -889,8 +889,8 @@
         <v>4</v>
       </c>
       <c r="F12" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>2</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -908,8 +908,8 @@
         <v>3</v>
       </c>
       <c r="F13" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1.5</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -927,8 +927,8 @@
         <v>1.5</v>
       </c>
       <c r="F14" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>0.75</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -946,8 +946,8 @@
         <v>2</v>
       </c>
       <c r="F15" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -965,8 +965,8 @@
         <v>2</v>
       </c>
       <c r="F16" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -984,8 +984,8 @@
         <v>2.75</v>
       </c>
       <c r="F17" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1.375</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1003,8 +1003,8 @@
         <v>3</v>
       </c>
       <c r="F18" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>1.5</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1013,8 +1013,8 @@
         <v>40.25</v>
       </c>
       <c r="F19" s="1">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/2</f>
-        <v>20.125</v>
+        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
+        <v>13.416666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final commit on split task
</commit_message>
<xml_diff>
--- a/doc/Projet_libre_decoupage_tache.xlsx
+++ b/doc/Projet_libre_decoupage_tache.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeyvo/EPITECH/Projet Libre/PBRaytracer/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D33D7FD-8296-6746-BD65-B6B10CC53136}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{30C83C2B-B3BC-A841-87C2-88F3122CAE37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="2000" windowWidth="18600" windowHeight="14560" xr2:uid="{39DAB752-344B-9C46-BDE4-193F0B1E6DAC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{39DAB752-344B-9C46-BDE4-193F0B1E6DAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>Nom</t>
   </si>
@@ -47,80 +47,125 @@
     <t>Charge de travail (en jour/Homme)</t>
   </si>
   <si>
-    <t>JSON Parser</t>
+    <t>BOUZIDI</t>
+  </si>
+  <si>
+    <t>Mohamed</t>
+  </si>
+  <si>
+    <t>Implémentation de petits outils comme une interface de debug</t>
+  </si>
+  <si>
+    <t>Outils</t>
+  </si>
+  <si>
+    <t>Implémentation d'une petite librairie mathématique (Vector, matrix, etc..)</t>
   </si>
   <si>
     <t>Math Librairie</t>
   </si>
   <si>
+    <t>Implémentation de la primitive sphère afin de pouvoir les afficher.</t>
+  </si>
+  <si>
     <t>Sphere</t>
   </si>
   <si>
+    <t>DUMONTET</t>
+  </si>
+  <si>
+    <t>Damien</t>
+  </si>
+  <si>
+    <t>Implémentation de la primitive rectangle afin de pouvoir les afficher.</t>
+  </si>
+  <si>
     <t>Rectangle</t>
   </si>
   <si>
+    <t>Implémentation d'un algo d'antialiasing</t>
+  </si>
+  <si>
     <t>Antialiasing</t>
   </si>
   <si>
+    <t>Implémentation de matériaux de type non métallique et non transparent. </t>
+  </si>
+  <si>
     <t>Diffuse material</t>
   </si>
   <si>
+    <t>Implémentation de matériaux de type métallique.</t>
+  </si>
+  <si>
+    <t>Metal material</t>
+  </si>
+  <si>
+    <t>Implémentation d’un système de scene.</t>
+  </si>
+  <si>
     <t>World Instance</t>
   </si>
   <si>
-    <t>Dielecctrics material</t>
-  </si>
-  <si>
-    <t>Metal material</t>
+    <t>Implémentation de matériaux de type verre.</t>
+  </si>
+  <si>
+    <t>Dielectrics material</t>
+  </si>
+  <si>
+    <t>Implémentation d’une camera de type pinhole.</t>
   </si>
   <si>
     <t>Camera</t>
   </si>
   <si>
+    <t>Implémentation de l'effet blur (flou, depth of field)</t>
+  </si>
+  <si>
     <t>Blur</t>
   </si>
   <si>
+    <t>implémentation de l'effet Motion blur (flou de mouvement)</t>
+  </si>
+  <si>
     <t>Motion Blur</t>
   </si>
   <si>
+    <t>Implémentation de texture sur nos primitives</t>
+  </si>
+  <si>
     <t>Texture</t>
   </si>
   <si>
+    <t>Implémentation d'un algo de perlin noise afin de générer des texture procédural</t>
+  </si>
+  <si>
     <t>Perlin Noise</t>
   </si>
   <si>
+    <t>Implémentation du texture mapping afin de mapper nos texture sur nos objets</t>
+  </si>
+  <si>
     <t>Texture Mapping</t>
   </si>
   <si>
+    <t>Implémentation de matériaux de type émission afin d'avoir différentes lumière dans nos scènes</t>
+  </si>
+  <si>
     <t>Light</t>
   </si>
   <si>
+    <t xml:space="preserve">Implémentation de matériaux de type volume afin d'avoir un système de fumée </t>
+  </si>
+  <si>
     <t>Volume</t>
-  </si>
-  <si>
-    <t>Mohamed</t>
-  </si>
-  <si>
-    <t>BOUZIDI</t>
-  </si>
-  <si>
-    <t>DUMONTET</t>
-  </si>
-  <si>
-    <t>Damien</t>
-  </si>
-  <si>
-    <t>Crédit</t>
-  </si>
-  <si>
-    <t>NOTE: 1 jour/Homme = 8h de travail; 3 jours/Homme = 1 crédit; 24h réel de travail = 1 credit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,15 +176,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -166,35 +202,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <b val="0"/>
@@ -335,17 +351,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C020A962-C6E1-0347-A587-050EA1D2ECFF}" name="Tableau3" displayName="Tableau3" ref="A1:F19" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F19" xr:uid="{CED272F3-0BDE-0D48-A9EB-F2F9419CBC03}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1527BB05-FDF1-0C49-84C7-17399836837E}" name="Nom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B3DE6880-0B98-4D4B-9E28-90EAD24504C2}" name="Prénom" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{BC550481-ECA8-5D42-9BE5-45AE52C157D6}" name="Partie du projet" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1C29566B-021E-4847-A43C-BA9A304594FB}" name="Tâche fonctionnelle" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{089EF323-C7BA-0F4F-AE31-612C56D94DBA}" name="Charge de travail (en jour/Homme)" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{98E21285-F6C2-5141-97EE-6DD5D126E215}" name="Crédit" dataDxfId="0">
-      <calculatedColumnFormula>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</calculatedColumnFormula>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C020A962-C6E1-0347-A587-050EA1D2ECFF}" name="Tableau3" displayName="Tableau3" ref="A1:E19" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E19" xr:uid="{CED272F3-0BDE-0D48-A9EB-F2F9419CBC03}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1527BB05-FDF1-0C49-84C7-17399836837E}" name="Nom" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B3DE6880-0B98-4D4B-9E28-90EAD24504C2}" name="Prénom" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{BC550481-ECA8-5D42-9BE5-45AE52C157D6}" name="Partie du projet" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1C29566B-021E-4847-A43C-BA9A304594FB}" name="Tâche fonctionnelle" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{089EF323-C7BA-0F4F-AE31-612C56D94DBA}" name="Charge de travail (en jour/Homme)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -648,373 +661,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A726377-1964-D341-8EAE-D95ECF1DA9DA}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="3" max="3" width="78.5" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3">
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2">
         <v>3</v>
       </c>
-      <c r="F6" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3">
-        <v>3</v>
-      </c>
-      <c r="F7" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3">
-        <v>3</v>
-      </c>
-      <c r="F8" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="3">
-        <v>4</v>
-      </c>
-      <c r="F12" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="3">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="F14" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="3">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="3">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="3">
-        <v>2.75</v>
-      </c>
-      <c r="F17" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>0.91666666666666663</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="3">
-        <v>3</v>
-      </c>
-      <c r="F18" s="3">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E19" s="1">
         <f>SUM(E2:E18)</f>
-        <v>40.25</v>
-      </c>
-      <c r="F19" s="1">
-        <f>Tableau3[[#This Row],[Charge de travail (en jour/Homme)]]/3</f>
-        <v>13.416666666666666</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>